<commit_message>
update title for login & report screen
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1749,14 +1749,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2123,7 +2123,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:E25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2141,18 +2141,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="E1" s="19"/>
+      <c r="I1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="19"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="10" t="s">
@@ -2586,30 +2586,30 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="B22" s="20"/>
+      <c r="B22" s="18"/>
       <c r="I22" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="20"/>
       <c r="I23" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
       <c r="I24" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
       <c r="I25" s="1" t="s">
         <v>123</v>
       </c>

</xml_diff>